<commit_message>
Refactor api endpoint validation
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -1644,7 +1644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2842,6 +2842,47 @@
         <v>400</v>
       </c>
       <c r="I29" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-03-05 13:29:35</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>400</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>400</v>
+      </c>
+      <c r="I30" t="n">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor config file handling
Refactor legacy code to follow modern practices.
Fix race condition in concurrent processing.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1753,6 +1753,47 @@
         <v>400</v>
       </c>
       <c r="I32" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-03-05 16:42:06</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>400</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>400</v>
+      </c>
+      <c r="I33" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1767,7 +1808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3088,6 +3129,47 @@
         <v>400</v>
       </c>
       <c r="I32" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-03-05 16:29:35</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>400</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>400</v>
+      </c>
+      <c r="I33" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3102,7 +3184,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4423,6 +4505,47 @@
         <v>400</v>
       </c>
       <c r="I32" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-03-05 16:51:45</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>400</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>400</v>
+      </c>
+      <c r="I33" t="n">
         <v>255</v>
       </c>
     </row>
@@ -4437,7 +4560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5761,6 +5884,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-03-05 16:41:15</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>400</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>400</v>
+      </c>
+      <c r="I33" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove logging system configuration
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1794,6 +1794,47 @@
         <v>400</v>
       </c>
       <c r="I33" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-03-05 17:42:06</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>400</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>400</v>
+      </c>
+      <c r="I34" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1808,7 +1849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3170,6 +3211,47 @@
         <v>400</v>
       </c>
       <c r="I33" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-03-05 17:29:35</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>400</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>400</v>
+      </c>
+      <c r="I34" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3184,7 +3266,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4546,6 +4628,47 @@
         <v>400</v>
       </c>
       <c r="I33" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-03-05 17:51:45</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>400</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>400</v>
+      </c>
+      <c r="I34" t="n">
         <v>255</v>
       </c>
     </row>
@@ -4560,7 +4683,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5925,6 +6048,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-03-05 17:41:15</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>400</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>400</v>
+      </c>
+      <c r="I34" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove config file handling
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1835,6 +1835,47 @@
         <v>400</v>
       </c>
       <c r="I34" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-03-05 18:42:06</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>400</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>400</v>
+      </c>
+      <c r="I35" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1849,7 +1890,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3252,6 +3293,47 @@
         <v>400</v>
       </c>
       <c r="I34" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-03-05 18:29:35</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>400</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>400</v>
+      </c>
+      <c r="I35" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3266,7 +3348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4669,6 +4751,47 @@
         <v>400</v>
       </c>
       <c r="I34" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-03-05 18:51:45</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>400</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>400</v>
+      </c>
+      <c r="I35" t="n">
         <v>255</v>
       </c>
     </row>
@@ -4683,7 +4806,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6089,6 +6212,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-03-05 18:41:15</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>400</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>400</v>
+      </c>
+      <c r="I35" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove responsive design implementation
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1876,6 +1876,47 @@
         <v>400</v>
       </c>
       <c r="I35" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-03-05 19:42:06</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>400</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>400</v>
+      </c>
+      <c r="I36" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1890,7 +1931,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3334,6 +3375,47 @@
         <v>400</v>
       </c>
       <c r="I35" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-03-05 19:29:35</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>400</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>400</v>
+      </c>
+      <c r="I36" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3348,7 +3430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4792,6 +4874,47 @@
         <v>400</v>
       </c>
       <c r="I35" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-03-05 19:51:45</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>400</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>400</v>
+      </c>
+      <c r="I36" t="n">
         <v>255</v>
       </c>
     </row>
@@ -4806,7 +4929,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6253,6 +6376,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-03-05 19:41:15</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>400</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>400</v>
+      </c>
+      <c r="I36" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert navigation menu accessibility
Address edge cases reported in user feedback.
Simplify code structure to improve readability.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1917,6 +1917,47 @@
         <v>400</v>
       </c>
       <c r="I36" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:42:06</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>400</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>400</v>
+      </c>
+      <c r="I37" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1931,7 +1972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3416,6 +3457,47 @@
         <v>400</v>
       </c>
       <c r="I36" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:29:35</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>400</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>400</v>
+      </c>
+      <c r="I37" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3430,7 +3512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4915,6 +4997,47 @@
         <v>400</v>
       </c>
       <c r="I36" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:51:45</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>400</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>400</v>
+      </c>
+      <c r="I37" t="n">
         <v>255</v>
       </c>
     </row>
@@ -4929,7 +5052,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6417,6 +6540,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-03-05 20:41:15</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>400</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>400</v>
+      </c>
+      <c r="I37" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix error message display
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1958,6 +1958,47 @@
         <v>400</v>
       </c>
       <c r="I37" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-03-05 21:42:06</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>400</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>400</v>
+      </c>
+      <c r="I38" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1972,7 +2013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3498,6 +3539,47 @@
         <v>400</v>
       </c>
       <c r="I37" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-03-05 21:29:35</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>400</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>400</v>
+      </c>
+      <c r="I38" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3512,7 +3594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5038,6 +5120,47 @@
         <v>400</v>
       </c>
       <c r="I37" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-03-05 21:51:45</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>400</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>400</v>
+      </c>
+      <c r="I38" t="n">
         <v>255</v>
       </c>
     </row>
@@ -5052,7 +5175,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6581,6 +6704,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-03-05 21:41:15</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>400</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>400</v>
+      </c>
+      <c r="I38" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove csv module error handling
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1999,6 +1999,47 @@
         <v>400</v>
       </c>
       <c r="I38" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-03-05 22:42:06</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>400</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>400</v>
+      </c>
+      <c r="I39" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2013,7 +2054,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3580,6 +3621,47 @@
         <v>400</v>
       </c>
       <c r="I38" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-03-05 22:29:35</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>400</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>400</v>
+      </c>
+      <c r="I39" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3594,7 +3676,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5161,6 +5243,47 @@
         <v>400</v>
       </c>
       <c r="I38" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-03-05 22:51:45</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>400</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>400</v>
+      </c>
+      <c r="I39" t="n">
         <v>255</v>
       </c>
     </row>
@@ -5175,7 +5298,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6745,6 +6868,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-03-05 22:41:15</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>400</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>400</v>
+      </c>
+      <c r="I39" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement security vulnerability checks
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2040,6 +2040,47 @@
         <v>400</v>
       </c>
       <c r="I39" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-03-05 23:42:06</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>400</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>400</v>
+      </c>
+      <c r="I40" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2054,7 +2095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3662,6 +3703,47 @@
         <v>400</v>
       </c>
       <c r="I39" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-03-05 23:29:35</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>400</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>400</v>
+      </c>
+      <c r="I40" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3676,7 +3758,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5284,6 +5366,47 @@
         <v>400</v>
       </c>
       <c r="I39" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-03-05 23:51:45</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>400</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>400</v>
+      </c>
+      <c r="I40" t="n">
         <v>255</v>
       </c>
     </row>
@@ -5298,7 +5421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6909,6 +7032,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-03-05 23:41:15</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>400</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>400</v>
+      </c>
+      <c r="I40" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix responsive design implementation
Add missing documentation for the new API.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2081,6 +2081,47 @@
         <v>400</v>
       </c>
       <c r="I40" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-03-06 00:42:06</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>400</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>400</v>
+      </c>
+      <c r="I41" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2095,7 +2136,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3744,6 +3785,47 @@
         <v>400</v>
       </c>
       <c r="I40" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-03-06 00:29:35</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>400</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>400</v>
+      </c>
+      <c r="I41" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3758,7 +3840,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5407,6 +5489,47 @@
         <v>400</v>
       </c>
       <c r="I40" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-03-06 00:51:45</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>400</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>400</v>
+      </c>
+      <c r="I41" t="n">
         <v>255</v>
       </c>
     </row>
@@ -5421,7 +5544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7073,6 +7196,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-03-06 00:41:15</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>400</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>400</v>
+      </c>
+      <c r="I41" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance image processing memory leaks
Apply code style fixes as per linter recommendations.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2204,6 +2204,47 @@
         <v>400</v>
       </c>
       <c r="I43" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-03-06 03:42:06</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>400</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>400</v>
+      </c>
+      <c r="I44" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2218,7 +2259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3990,6 +4031,47 @@
         <v>400</v>
       </c>
       <c r="I43" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-03-06 03:29:35</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>400</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>400</v>
+      </c>
+      <c r="I44" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4004,7 +4086,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5776,6 +5858,47 @@
         <v>400</v>
       </c>
       <c r="I43" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-03-06 03:51:45</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>400</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>400</v>
+      </c>
+      <c r="I44" t="n">
         <v>255</v>
       </c>
     </row>
@@ -5790,7 +5913,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7565,6 +7688,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-03-06 03:41:15</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>400</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>400</v>
+      </c>
+      <c r="I44" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove user authentication module
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2245,6 +2245,47 @@
         <v>400</v>
       </c>
       <c r="I44" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-03-06 04:42:06</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>400</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>400</v>
+      </c>
+      <c r="I45" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2259,7 +2300,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4072,6 +4113,47 @@
         <v>400</v>
       </c>
       <c r="I44" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-03-06 04:29:35</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>400</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>400</v>
+      </c>
+      <c r="I45" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4086,7 +4168,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5899,6 +5981,47 @@
         <v>400</v>
       </c>
       <c r="I44" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-03-06 04:51:45</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>400</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>400</v>
+      </c>
+      <c r="I45" t="n">
         <v>255</v>
       </c>
     </row>
@@ -5913,7 +6036,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7729,6 +7852,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-03-06 04:41:15</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>400</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>400</v>
+      </c>
+      <c r="I45" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix file upload functionality
Correct null value handling in data processing.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2286,6 +2286,47 @@
         <v>400</v>
       </c>
       <c r="I45" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-03-06 05:42:06</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>400</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>400</v>
+      </c>
+      <c r="I46" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2300,7 +2341,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4154,6 +4195,47 @@
         <v>400</v>
       </c>
       <c r="I45" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-03-06 05:29:35</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>400</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>400</v>
+      </c>
+      <c r="I46" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4168,7 +4250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6022,6 +6104,47 @@
         <v>400</v>
       </c>
       <c r="I45" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-03-06 05:51:45</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>400</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>400</v>
+      </c>
+      <c r="I46" t="n">
         <v>255</v>
       </c>
     </row>
@@ -6036,7 +6159,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7893,6 +8016,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-03-06 05:41:15</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>400</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>400</v>
+      </c>
+      <c r="I46" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update login page ui elements
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2368,6 +2368,47 @@
         <v>400</v>
       </c>
       <c r="I47" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-03-06 07:42:06</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>400</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>400</v>
+      </c>
+      <c r="I48" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2382,7 +2423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4318,6 +4359,47 @@
         <v>400</v>
       </c>
       <c r="I47" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-03-06 07:29:35</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>400</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>400</v>
+      </c>
+      <c r="I48" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4332,7 +4414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6268,6 +6350,47 @@
         <v>400</v>
       </c>
       <c r="I47" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-03-06 07:51:45</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>400</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>400</v>
+      </c>
+      <c r="I48" t="n">
         <v>255</v>
       </c>
     </row>
@@ -6282,7 +6405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8221,6 +8344,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-03-06 07:41:15</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>400</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>400</v>
+      </c>
+      <c r="I48" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance user authentication module
Address edge cases reported in user feedback.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2409,6 +2409,47 @@
         <v>400</v>
       </c>
       <c r="I48" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-03-06 08:42:06</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>400</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>400</v>
+      </c>
+      <c r="I49" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2423,7 +2464,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4400,6 +4441,47 @@
         <v>400</v>
       </c>
       <c r="I48" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-03-06 08:29:35</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>400</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>400</v>
+      </c>
+      <c r="I49" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4414,7 +4496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6391,6 +6473,47 @@
         <v>400</v>
       </c>
       <c r="I48" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-03-06 08:51:45</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>400</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>400</v>
+      </c>
+      <c r="I49" t="n">
         <v>255</v>
       </c>
     </row>
@@ -6405,7 +6528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8385,6 +8508,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-03-06 08:41:15</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>400</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>400</v>
+      </c>
+      <c r="I49" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify error message display
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2450,6 +2450,47 @@
         <v>400</v>
       </c>
       <c r="I49" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-03-06 09:42:06</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>400</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>400</v>
+      </c>
+      <c r="I50" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2464,7 +2505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4482,6 +4523,47 @@
         <v>400</v>
       </c>
       <c r="I49" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-03-06 09:29:35</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>400</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>400</v>
+      </c>
+      <c r="I50" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4496,7 +4578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6514,6 +6596,47 @@
         <v>400</v>
       </c>
       <c r="I49" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-03-06 09:51:45</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>400</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>400</v>
+      </c>
+      <c r="I50" t="n">
         <v>255</v>
       </c>
     </row>
@@ -6528,7 +6651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8549,6 +8672,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-03-06 09:41:15</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>400</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>400</v>
+      </c>
+      <c r="I50" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data parsing logic
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2491,6 +2491,47 @@
         <v>400</v>
       </c>
       <c r="I50" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-03-06 10:42:06</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>400</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>400</v>
+      </c>
+      <c r="I51" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2505,7 +2546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4564,6 +4605,47 @@
         <v>400</v>
       </c>
       <c r="I50" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-03-06 10:29:35</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>400</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>400</v>
+      </c>
+      <c r="I51" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4578,7 +4660,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6637,6 +6719,47 @@
         <v>400</v>
       </c>
       <c r="I50" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-03-06 10:51:45</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>400</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>400</v>
+      </c>
+      <c r="I51" t="n">
         <v>255</v>
       </c>
     </row>
@@ -6651,7 +6774,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8713,6 +8836,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-03-06 10:41:15</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>400</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>400</v>
+      </c>
+      <c r="I51" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance csv module error handling
Update dependencies to their latest versions.
Apply code style fixes as per linter recommendations.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2532,6 +2532,47 @@
         <v>400</v>
       </c>
       <c r="I51" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-03-06 11:42:06</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>400</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>400</v>
+      </c>
+      <c r="I52" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2546,7 +2587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4646,6 +4687,47 @@
         <v>400</v>
       </c>
       <c r="I51" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-03-06 11:29:35</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>400</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>400</v>
+      </c>
+      <c r="I52" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4660,7 +4742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6760,6 +6842,47 @@
         <v>400</v>
       </c>
       <c r="I51" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-03-06 11:51:45</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>400</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>400</v>
+      </c>
+      <c r="I52" t="n">
         <v>255</v>
       </c>
     </row>
@@ -6774,7 +6897,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8877,6 +9000,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-03-06 11:41:15</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>400</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>400</v>
+      </c>
+      <c r="I52" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add api endpoint validation
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2614,6 +2614,47 @@
         <v>400</v>
       </c>
       <c r="I53" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-03-06 13:42:06</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>400</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>400</v>
+      </c>
+      <c r="I54" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2628,7 +2669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4810,6 +4851,47 @@
         <v>400</v>
       </c>
       <c r="I53" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-03-06 13:29:35</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>400</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>400</v>
+      </c>
+      <c r="I54" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4824,7 +4906,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7006,6 +7088,47 @@
         <v>400</v>
       </c>
       <c r="I53" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-03-06 13:51:45</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>400</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>400</v>
+      </c>
+      <c r="I54" t="n">
         <v>255</v>
       </c>
     </row>
@@ -7020,7 +7143,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9205,6 +9328,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-03-06 13:41:15</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>400</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>400</v>
+      </c>
+      <c r="I54" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix user authentication module
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2696,6 +2696,47 @@
         <v>400</v>
       </c>
       <c r="I55" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-03-06 15:42:06</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>400</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>400</v>
+      </c>
+      <c r="I56" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2710,7 +2751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4974,6 +5015,47 @@
         <v>400</v>
       </c>
       <c r="I55" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-03-06 15:29:35</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>400</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>400</v>
+      </c>
+      <c r="I56" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4988,7 +5070,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7252,6 +7334,47 @@
         <v>400</v>
       </c>
       <c r="I55" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-03-06 15:51:45</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>400</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>400</v>
+      </c>
+      <c r="I56" t="n">
         <v>255</v>
       </c>
     </row>
@@ -7266,7 +7389,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9533,6 +9656,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-03-06 15:41:15</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>400</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>400</v>
+      </c>
+      <c r="I56" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance logging system configuration
Refactor legacy code to follow modern practices.
Address edge cases reported in user feedback.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2737,6 +2737,47 @@
         <v>400</v>
       </c>
       <c r="I56" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-03-06 16:42:06</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>400</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>400</v>
+      </c>
+      <c r="I57" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2751,7 +2792,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5056,6 +5097,47 @@
         <v>400</v>
       </c>
       <c r="I56" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-03-06 16:29:35</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>400</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>400</v>
+      </c>
+      <c r="I57" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5070,7 +5152,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7375,6 +7457,47 @@
         <v>400</v>
       </c>
       <c r="I56" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-03-06 16:51:45</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>400</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>400</v>
+      </c>
+      <c r="I57" t="n">
         <v>255</v>
       </c>
     </row>
@@ -7389,7 +7512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9697,6 +9820,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-03-06 16:41:15</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>400</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>400</v>
+      </c>
+      <c r="I57" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert logging system configuration
Refactor legacy code to follow modern practices.
Update dependencies to their latest versions.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2819,6 +2819,47 @@
         <v>400</v>
       </c>
       <c r="I58" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-03-06 18:42:06</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>400</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>400</v>
+      </c>
+      <c r="I59" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2833,7 +2874,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5220,6 +5261,47 @@
         <v>400</v>
       </c>
       <c r="I58" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-03-06 18:29:35</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>400</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>400</v>
+      </c>
+      <c r="I59" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5234,7 +5316,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7621,6 +7703,47 @@
         <v>400</v>
       </c>
       <c r="I58" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-03-06 18:51:45</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>400</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>400</v>
+      </c>
+      <c r="I59" t="n">
         <v>255</v>
       </c>
     </row>
@@ -7635,7 +7758,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10025,6 +10148,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-03-06 18:41:15</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>400</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>400</v>
+      </c>
+      <c r="I59" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade api endpoint validation
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2860,6 +2860,47 @@
         <v>400</v>
       </c>
       <c r="I59" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-03-06 19:42:06</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>400</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>400</v>
+      </c>
+      <c r="I60" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2874,7 +2915,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5302,6 +5343,47 @@
         <v>400</v>
       </c>
       <c r="I59" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-03-06 19:29:35</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>400</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>400</v>
+      </c>
+      <c r="I60" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5316,7 +5398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7744,6 +7826,47 @@
         <v>400</v>
       </c>
       <c r="I59" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-03-06 19:51:45</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>400</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>400</v>
+      </c>
+      <c r="I60" t="n">
         <v>255</v>
       </c>
     </row>
@@ -7758,7 +7881,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10189,6 +10312,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-03-06 19:41:15</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>400</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>400</v>
+      </c>
+      <c r="I60" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve navigation menu accessibility
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2901,6 +2901,47 @@
         <v>400</v>
       </c>
       <c r="I60" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-03-06 20:42:06</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>400</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>400</v>
+      </c>
+      <c r="I61" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2915,7 +2956,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5384,6 +5425,47 @@
         <v>400</v>
       </c>
       <c r="I60" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-03-06 20:29:35</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>400</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>400</v>
+      </c>
+      <c r="I61" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5398,7 +5480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7867,6 +7949,47 @@
         <v>400</v>
       </c>
       <c r="I60" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-03-06 20:51:45</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>400</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>400</v>
+      </c>
+      <c r="I61" t="n">
         <v>255</v>
       </c>
     </row>
@@ -7881,7 +8004,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10353,6 +10476,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-03-06 20:41:15</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>400</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>400</v>
+      </c>
+      <c r="I61" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade responsive design implementation
Update dependencies to their latest versions.
Address edge cases reported in user feedback.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2942,6 +2942,47 @@
         <v>400</v>
       </c>
       <c r="I61" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-03-06 21:42:06</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>400</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>400</v>
+      </c>
+      <c r="I62" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2956,7 +2997,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5466,6 +5507,47 @@
         <v>400</v>
       </c>
       <c r="I61" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-03-06 21:29:35</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>400</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>400</v>
+      </c>
+      <c r="I62" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5480,7 +5562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7990,6 +8072,47 @@
         <v>400</v>
       </c>
       <c r="I61" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-03-06 21:51:45</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>400</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>400</v>
+      </c>
+      <c r="I62" t="n">
         <v>255</v>
       </c>
     </row>
@@ -8004,7 +8127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10517,6 +10640,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-03-06 21:41:15</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>400</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>400</v>
+      </c>
+      <c r="I62" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify database schema migration
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2983,6 +2983,47 @@
         <v>400</v>
       </c>
       <c r="I62" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-03-06 22:42:06</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>400</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>400</v>
+      </c>
+      <c r="I63" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2997,7 +3038,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5548,6 +5589,47 @@
         <v>400</v>
       </c>
       <c r="I62" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-03-06 22:29:35</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>400</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>400</v>
+      </c>
+      <c r="I63" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5562,7 +5644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8113,6 +8195,47 @@
         <v>400</v>
       </c>
       <c r="I62" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-03-06 22:51:45</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>400</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>400</v>
+      </c>
+      <c r="I63" t="n">
         <v>255</v>
       </c>
     </row>
@@ -8127,7 +8250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10681,6 +10804,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-03-06 22:41:15</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>400</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>400</v>
+      </c>
+      <c r="I63" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve database schema migration
Add missing documentation for the new API.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3024,6 +3024,47 @@
         <v>400</v>
       </c>
       <c r="I63" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-03-06 23:42:06</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>400</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>400</v>
+      </c>
+      <c r="I64" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3038,7 +3079,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5630,6 +5671,47 @@
         <v>400</v>
       </c>
       <c r="I63" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-03-06 23:29:35</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>400</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>400</v>
+      </c>
+      <c r="I64" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5644,7 +5726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8236,6 +8318,47 @@
         <v>400</v>
       </c>
       <c r="I63" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-03-06 23:51:45</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>400</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>400</v>
+      </c>
+      <c r="I64" t="n">
         <v>255</v>
       </c>
     </row>
@@ -8250,7 +8373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10845,6 +10968,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-03-06 23:41:15</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>400</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>400</v>
+      </c>
+      <c r="I64" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade build script optimization
Update dependencies to their latest versions.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3065,6 +3065,47 @@
         <v>400</v>
       </c>
       <c r="I64" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-03-07 00:42:06</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>400</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>400</v>
+      </c>
+      <c r="I65" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3079,7 +3120,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5712,6 +5753,47 @@
         <v>400</v>
       </c>
       <c r="I64" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-03-07 00:29:35</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>400</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>400</v>
+      </c>
+      <c r="I65" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5726,7 +5808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8359,6 +8441,47 @@
         <v>400</v>
       </c>
       <c r="I64" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-03-07 00:51:45</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>400</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>400</v>
+      </c>
+      <c r="I65" t="n">
         <v>255</v>
       </c>
     </row>
@@ -8373,7 +8496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11009,6 +11132,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-03-07 00:41:15</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>400</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>400</v>
+      </c>
+      <c r="I65" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjust navigation menu accessibility
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3147,6 +3147,47 @@
         <v>400</v>
       </c>
       <c r="I66" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-03-07 02:42:06</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>400</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>400</v>
+      </c>
+      <c r="I67" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3161,7 +3202,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5876,6 +5917,47 @@
         <v>400</v>
       </c>
       <c r="I66" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-03-07 02:29:35</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>400</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>400</v>
+      </c>
+      <c r="I67" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5890,7 +5972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8605,6 +8687,47 @@
         <v>400</v>
       </c>
       <c r="I66" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-03-07 02:51:45</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>400</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>400</v>
+      </c>
+      <c r="I67" t="n">
         <v>255</v>
       </c>
     </row>
@@ -8619,7 +8742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11337,6 +11460,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-03-07 02:41:15</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>400</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>400</v>
+      </c>
+      <c r="I67" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise navigation menu accessibility
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3188,6 +3188,47 @@
         <v>400</v>
       </c>
       <c r="I67" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-03-07 03:42:06</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>400</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>400</v>
+      </c>
+      <c r="I68" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3202,7 +3243,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5958,6 +5999,47 @@
         <v>400</v>
       </c>
       <c r="I67" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-03-07 03:29:35</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>400</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>400</v>
+      </c>
+      <c r="I68" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5972,7 +6054,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8728,6 +8810,47 @@
         <v>400</v>
       </c>
       <c r="I67" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-03-07 03:51:45</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>400</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>400</v>
+      </c>
+      <c r="I68" t="n">
         <v>255</v>
       </c>
     </row>
@@ -8742,7 +8865,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11501,6 +11624,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-03-07 03:41:15</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>400</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>400</v>
+      </c>
+      <c r="I68" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor unit test coverage
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3229,6 +3229,47 @@
         <v>400</v>
       </c>
       <c r="I68" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-03-07 04:42:06</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>400</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>400</v>
+      </c>
+      <c r="I69" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3243,7 +3284,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6040,6 +6081,47 @@
         <v>400</v>
       </c>
       <c r="I68" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-03-07 04:29:35</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>400</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>400</v>
+      </c>
+      <c r="I69" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6054,7 +6136,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8851,6 +8933,47 @@
         <v>400</v>
       </c>
       <c r="I68" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-03-07 04:51:45</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>400</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>400</v>
+      </c>
+      <c r="I69" t="n">
         <v>255</v>
       </c>
     </row>
@@ -8865,7 +8988,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11665,6 +11788,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-03-07 04:41:15</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>400</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>400</v>
+      </c>
+      <c r="I69" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert csv module error handling
Simplify code structure to improve readability.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3311,6 +3311,47 @@
         <v>400</v>
       </c>
       <c r="I70" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-03-07 06:42:06</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>400</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>400</v>
+      </c>
+      <c r="I71" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3325,7 +3366,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6204,6 +6245,47 @@
         <v>400</v>
       </c>
       <c r="I70" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-03-07 06:29:35</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>400</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>400</v>
+      </c>
+      <c r="I71" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6218,7 +6300,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9097,6 +9179,47 @@
         <v>400</v>
       </c>
       <c r="I70" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-03-07 06:51:45</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>400</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>400</v>
+      </c>
+      <c r="I71" t="n">
         <v>255</v>
       </c>
     </row>
@@ -9111,7 +9234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11993,6 +12116,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-03-07 06:41:15</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>400</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>400</v>
+      </c>
+      <c r="I71" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement responsive design implementation
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3475,6 +3475,47 @@
         <v>400</v>
       </c>
       <c r="I74" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-03-07 10:42:06</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>400</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>400</v>
+      </c>
+      <c r="I75" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3489,7 +3530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6532,6 +6573,47 @@
         <v>400</v>
       </c>
       <c r="I74" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-03-07 10:29:35</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>400</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>400</v>
+      </c>
+      <c r="I75" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6546,7 +6628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9589,6 +9671,47 @@
         <v>400</v>
       </c>
       <c r="I74" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-03-07 10:51:45</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>400</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>400</v>
+      </c>
+      <c r="I75" t="n">
         <v>255</v>
       </c>
     </row>
@@ -9603,7 +9726,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12649,6 +12772,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-03-07 10:41:15</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>400</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>400</v>
+      </c>
+      <c r="I75" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade config file handling
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3516,6 +3516,47 @@
         <v>400</v>
       </c>
       <c r="I75" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-03-07 11:42:06</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>400</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>400</v>
+      </c>
+      <c r="I76" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3530,7 +3571,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6614,6 +6655,47 @@
         <v>400</v>
       </c>
       <c r="I75" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-03-07 11:29:35</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>400</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>400</v>
+      </c>
+      <c r="I76" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6628,7 +6710,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9712,6 +9794,47 @@
         <v>400</v>
       </c>
       <c r="I75" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-03-07 11:51:45</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>400</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>400</v>
+      </c>
+      <c r="I76" t="n">
         <v>255</v>
       </c>
     </row>
@@ -9726,7 +9849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12813,6 +12936,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-03-07 11:41:15</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>400</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>400</v>
+      </c>
+      <c r="I76" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct responsive design implementation
Improve performance by optimizing database queries.
Fix race condition in concurrent processing.
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3598,6 +3598,47 @@
         <v>400</v>
       </c>
       <c r="I77" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-03-07 13:42:06</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>400</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H78" t="n">
+        <v>400</v>
+      </c>
+      <c r="I78" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3612,7 +3653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6778,6 +6819,47 @@
         <v>400</v>
       </c>
       <c r="I77" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-03-07 13:29:35</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>400</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H78" t="n">
+        <v>400</v>
+      </c>
+      <c r="I78" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6792,7 +6874,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9958,6 +10040,47 @@
         <v>400</v>
       </c>
       <c r="I77" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-03-07 13:51:45</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>400</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H78" t="n">
+        <v>400</v>
+      </c>
+      <c r="I78" t="n">
         <v>255</v>
       </c>
     </row>
@@ -9972,7 +10095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13141,6 +13264,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-03-07 13:41:15</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>400</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H78" t="n">
+        <v>400</v>
+      </c>
+      <c r="I78" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix config file handling
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3803,6 +3803,47 @@
         <v>400</v>
       </c>
       <c r="I82" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-03-07 18:42:06</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>400</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H83" t="n">
+        <v>400</v>
+      </c>
+      <c r="I83" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3817,7 +3858,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7188,6 +7229,47 @@
         <v>400</v>
       </c>
       <c r="I82" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-03-07 18:29:35</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>400</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H83" t="n">
+        <v>400</v>
+      </c>
+      <c r="I83" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7202,7 +7284,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10573,6 +10655,47 @@
         <v>400</v>
       </c>
       <c r="I82" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-03-07 18:51:45</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>400</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H83" t="n">
+        <v>400</v>
+      </c>
+      <c r="I83" t="n">
         <v>255</v>
       </c>
     </row>
@@ -10587,7 +10710,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13961,6 +14084,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-03-07 18:41:15</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>400</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H83" t="n">
+        <v>400</v>
+      </c>
+      <c r="I83" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance responsive design implementation
</commit_message>
<xml_diff>
--- a/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
+++ b/SAG1_sensor_data_with_decimal_filtered_updated.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3885,6 +3885,47 @@
         <v>400</v>
       </c>
       <c r="I84" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-03-07 20:42:06</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>0x d</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>400</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>568631262647113770877196</t>
+        </is>
+      </c>
+      <c r="H85" t="n">
+        <v>400</v>
+      </c>
+      <c r="I85" t="n">
         <v>13</v>
       </c>
     </row>
@@ -3899,7 +3940,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7352,6 +7393,47 @@
         <v>400</v>
       </c>
       <c r="I84" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-03-07 20:29:35</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>0x e</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>400</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>568631262647113770942732</t>
+        </is>
+      </c>
+      <c r="H85" t="n">
+        <v>400</v>
+      </c>
+      <c r="I85" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7366,7 +7448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10819,6 +10901,47 @@
         <v>400</v>
       </c>
       <c r="I84" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-03-07 20:51:45</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>400</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H85" t="n">
+        <v>400</v>
+      </c>
+      <c r="I85" t="n">
         <v>255</v>
       </c>
     </row>
@@ -10833,7 +10956,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14289,6 +14412,47 @@
         <v>3</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-03-07 20:41:15</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0x01,0x90 </t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>0x 3</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>400</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>568631262647113769959692</t>
+        </is>
+      </c>
+      <c r="H85" t="n">
+        <v>400</v>
+      </c>
+      <c r="I85" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>